<commit_message>
- Implementado envio de email com anexo.
</commit_message>
<xml_diff>
--- a/data/jobs_information.xlsx
+++ b/data/jobs_information.xlsx
@@ -556,10 +556,47 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>UI Path - RPA Developer</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Role : UI Path_RPA Developer
+Location : 100% remote
+Job Description</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Human Resources</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>RPA Developer</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Description
 "You've worked for the rest...now work for the best!"
@@ -572,37 +609,37 @@
 "Veteran Friendly"</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Entry level</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Renewable Energy Semiconductor Manufacturing</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>RPA Analyst</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Company Description
 ClientSolv Technologies is an IT solution firm with over a decade of experience serving Fortune 1000 companies, public sector and small to medium sized companies. ClientSolv Technologies is a woman-owned and operated company that is certified as a WMBE, 8a firm by the Federal government's Small Business Administration.
@@ -612,37 +649,37 @@
 Additional Information</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>IT Services and IT Consulting</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>RPA Analyst</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Company Description
 ClientSolv Technologies is an IT solution firm with over a decade of experience serving Fortune 1000 companies, public sector and small to medium sized companies. ClientSolv Technologies is a woman-owned and operated company that is certified as a WMBE, 8a firm by the Federal government's Small Business Administration.
@@ -652,37 +689,37 @@
 Additional Information</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>IT Services and IT Consulting</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>RPA Product &amp; Engineering Lead</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>At Disney, we’re storytellers. We make the impossible, possible. The Walt Disney Company is a world-class entertainment and technological leader. Walt’s passion was to continuously envision new ways to move audiences around the world—a passion that remains our touchstone in an enterprise that stretches from theme parks, resorts and a cruise line to sports, news, movies and a variety of other businesses. Uniting each endeavor is a commitment to creating and delivering unforgettable experiences — and we’re constantly looking for new ways to enhance these exciting experiences.
 The Enterprise Technology mission is to deliver technology solutions that align to business strategies while enabling enterprise efficiency and promoting cross-company collaborative innovation. The Enterprise Technology organization drives competitive advantage by enhancing our consumer experiences, enabling business growth, and advancing operational excellence.
@@ -691,37 +728,37 @@
 The hiring range for this position in California is $149,240 to $200,200 per year and in Washington State is $156,292 to $209,660 per year. The base pay actually offered will take into account internal equity and also may vary depending on the candidate’s geographic region, job-related knowledge, skills, and experience among other factors. A bonus and/or long-term incentive units may be provided as part of the compensation package, in addition to the full range of medical, financial, and/or other benefits, dependent on the level and position offered.</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Entertainment Providers</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>RPA Consultant</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Job Description
 Role RPA Consultant
@@ -741,51 +778,14 @@
 Added experience of using Python for Web development frameworks is a plus.</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>RPA Consultant</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Job Description
-RPA Consultant
-Hockessin, DE</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Contract</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -809,82 +809,6 @@
         </is>
       </c>
       <c r="C10" t="inlineStr">
-        <is>
-          <t>Job Description
-Role: RPA Consultant
-Location: Austin, TX
-Experience: 4-6 Year
-Duration: 6-12 Months</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RPA CONSULTANT</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Job Description
-RPA Consultant
-Syracuse, NY</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>RPA Consultant</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
         <is>
           <t>Job Description
 Role RPA Consultant
@@ -904,6 +828,82 @@
 Added experience of using Python for Web development frameworks is a plus.</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Mid-Senior level</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RPA Consultant</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Job Description
+RPA Consultant
+Hockessin, DE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Mid-Senior level</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Contract</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>RPA Consultant</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Job Description
+Role: RPA Consultant
+Location: Austin, TX
+Experience: 4-6 Year
+Duration: 6-12 Months</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
@@ -911,7 +911,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -931,33 +931,34 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RPA Technical Analyst</t>
+          <t>RPA CONSULTANT</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>We are seeking a Robotic Process Automation (RPA) Technical Analyst to join a larger team that supports our Federal customer in the identification and automation of Momentum processes. The RPA Technical Analyst will follow the full lifecycle of development and deployment of processes to be automated. Candidates should have familiarity with Federal financials, experience with Momentum is preferred. This is a full-time position on a multi-year contract that will allow for remote work with occasional on-site client meetings in Washington, DC.
-All employment decisions shall be made without regard to age, race, creed, color, religion, sex, national origin, ancestry, disability status, veteran status, sexual orientation, gender identity or expression, genetic information, marital status, citizenship status or any other basis as protected by federal, state, or local law.</t>
+          <t>Job Description
+RPA Consultant
+Syracuse, NY</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Entry level</t>
+          <t>Mid-Senior level</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Engineering and Information Technology</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Technology, Information and Internet</t>
+          <t>Software Development</t>
         </is>
       </c>
     </row>
@@ -967,47 +968,83 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>RPA Technical Analyst</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>We are seeking a Robotic Process Automation (RPA) Technical Analyst to join a larger team that supports our Federal customer in the identification and automation of Momentum processes. The RPA Technical Analyst will follow the full lifecycle of development and deployment of processes to be automated. Candidates should have familiarity with Federal financials, experience with Momentum is preferred. This is a full-time position on a multi-year contract that will allow for remote work with occasional on-site client meetings in Washington, DC.
+All employment decisions shall be made without regard to age, race, creed, color, religion, sex, national origin, ancestry, disability status, veteran status, sexual orientation, gender identity or expression, genetic information, marital status, citizenship status or any other basis as protected by federal, state, or local law.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Information Technology</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Technology, Information and Internet</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>RPA Engineer</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Job Description
 Title: RPA Engineer
 Location: New York, NY</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Entry level</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Contract</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>Software Development</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>RPA (Robotic Process Automation)</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Job Description
 !! Greetings !!
@@ -1019,37 +1056,37 @@
 Excellent communication skills both verbal and written, and comfortable presenting materials across multiple levels of the organization. Must have strong technical knowledge and analytical skills.</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Entry level</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>Software Development</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Remote UiPath Robotics Process Automation Engineer (RPA) - Remote | WFH</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Are you ready to join a dynamic team and revolutionize the way our government customer/MBS provider agency operates? We're looking for a talented RPA Engineer to develop cutting-edge Robotic Process Automation (RPA) solutions, including Artificial Intelligence (AI), Cognitive Computing/Machine Learning (ML), and Chatbots. In this role, you'll have the opportunity to work in an agile software development environment and make a real impact.
 As an RPA Engineer, you will be responsible for supporting the development and management of all operational bots. You'll assess the suitability of use cases and optimize processes, develop and test bots, provide chatbot proof-of-concepts, and monitor the performance and security of the digital workforce.
@@ -1062,37 +1099,37 @@
 So, are you ready to take on this exciting challenge and make a difference? Apply now!</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Entry level</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>Human Resources Services</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>RPA PM</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Job Description
 Job Title: RPO PM
@@ -1100,37 +1137,37 @@
 Duration: Contract-to-Hire</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Entry level</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
         <is>
           <t>Project Management and Information Technology</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Software Development</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>RPA PM</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>Job Description
 RPA PM
@@ -1138,37 +1175,119 @@
 The PM position requires and MAPD knowledge is nice to have.</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Entry level</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>Contract</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>Project Management and Information Technology</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Software Development</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Automation Engineer</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Job Details
+Description
+About Canal Insurance
+Canal Insurance Company was founded in 1939 and is located in Greenville, South Carolina. Canal specializes in insurance for commercial trucking and specialty transportation operations. While Canal does not write insurance in all states, the claims department handles claims in all 48 contiguous states and Canada. Canal’s customers are mainly federally regulated Motor Carriers and as such the core group of customers carry $1,000,000 in liability limits.
+At Canal, we recognize that our success would not be possible without the hard work and dedication of our employees. We know that happiness and productivity go hand in hand, and to that end, we consciously cultivate a culture that enables us to recruit and retain the very best talent in the business.
+The Automation Engineer will be responsible for designing, developing, and implementing automation solutions to improve efficiency and productivity in the development, testing, and deployment of software applications. You will also work with IT and Business cross-functional teams to identify opportunities for automation and implement solutions to meet those needs.
+Bachelor’s degree in business, computer science, engineering or related field, or related years of experience
+Constant use of vision, hearing, and communication (oral and written in person and via telephone). Frequent concentration, standing, walking, handling, reaching, and grasping. Occasional bending, kneeling and lifting (up to 25 lbs.) Heavy use of computer and office equipment.
+Occasional travel may be required. Periodic work outside of standard business hours or on weekends may be required.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Insurance</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>UIPath Developer - RPA Developer</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Position: UIPath Developer - RPA Developer
+Location: Alameda, CA ( onsite only)
+Position Type: Full-time Employee or contract
+Be a part of the Operations team focusing on Robotics process automation maintenance Monitoring RPA tool (UiPath)
+We offer a competitive salary, benefits, and a dynamic work environment. If you have a passion for technology and are looking for an exciting opportunity to work with a talented team, please apply today</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Contract</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Information Technology &amp; Services</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>RPA BA</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>Job Description
 Role: RPA BA
@@ -1189,37 +1308,37 @@
 Configuration setup, end-to-end testing, and maintenance of RPA, Finance and Legal systems /applications</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t>Research, Analyst, and Information Technology</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Software Development</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>RPA BA</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>Job Description
 Role: RPA BA
@@ -1241,37 +1360,37 @@
 Configuration setup, end-to-end testing, and maintenance of RPA, Finance and Legal systems /applications</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Contract</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Research, Analyst, and Information Technology</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>Software Development</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>RPA BA</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Job Description
 RPA BA
@@ -1279,37 +1398,37 @@
 Contract</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>Contract</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>Research, Analyst, and Information Technology</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>Software Development</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>Robotic Process Automation (RPA) BA</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Job Description
 Role Robotic Process Automation (RPA) BA
@@ -1317,150 +1436,24 @@
 Duration 6 months (Contract to hire after 6 months)</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Entry level</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>UIPath Developer - RPA Developer</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Position: UIPath Developer - RPA Developer
-Location: Alameda, CA ( onsite only)
-Position Type: Full-time Employee or contract
-Be a part of the Operations team focusing on Robotics process automation maintenance Monitoring RPA tool (UiPath)
-We offer a competitive salary, benefits, and a dynamic work environment. If you have a passion for technology and are looking for an exciting opportunity to work with a talented team, please apply today</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Entry level</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Information Technology &amp; Services</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>RPA SOFTWARE DEVELOPER</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Purpose Of Position
-The primary purpose of the RPA Software Developer is to work with the Artificial Intelligence automation team to develop processes, perform machine learning and automate tasks which were previously manual.
-The above statements reflect the general duties considered necessary to describe the principle functions of the job as identified, and are not a detailed description of all the work requirements that may be inherent to this position.
-All qualified applicants will receive consideration for employment without regard to race, color, religion, sex, gender identity, sexual orientation, age, national origin, disability, or protected veteran status. AultCare is an EEO/AA Employer M/F/Disability/Vet.
-AultCare/AHF will provide reasonable accommodations to employees or applicants with disabilities, as defined by the Americans with Disabilities Act, who are otherwise qualified to safely perform the essential functions of the job, with or without accommodation, unless such accommodation would constitute an undue hardship on AultCare/AHF or poses a direct threat to the health and safety of the individual or others that cannot be sufficiently mitigated by reasonable accommodation. Any applicant or employee who requires an accommodation to perform the essential functions of his or her job or to enjoy equal benefits and privileges of employment should notify the AultCare Human Resource Department and request such an accommodation.</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Entry level</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Hospitals and Health Care</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>RPA Lead (Remote)</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Job Description:
-About the Position:
-Title: RPA Lead
-Senior Manager – Business Engagement
-Remote eligible – must be in Eastern or Central time zone
-The RPA Lead will be a leading role in our Robotic Process Automation Team. They will work closely with Finance and Shared Services teams for all their automation initiatives and participate in all the phases of automations. This includes planning, application and solution design, development of custom solutions with the help of third-party vendors, application integration, and monitoring.
-The salary range for this position is $100,000.00 - 120,000.00 USD. The salary range may be higher or lower depending on the applicant’s location. All eligible Team Members will be offered health insurance (medical, dental, vision, Rx), life insurance, accidental death &amp; dismemberment (AD&amp;D), short-term and long-term disability, extended leave options, paid time off, company holidays, 401k matching, employee stock purchase plan, legal assistance, wellness programs, tuition reimbursement and discount programs.
-If you are interested in an open position but feel you may not meet all the listed qualifications, we still encourage you to apply.
-At Terex, we fully embrace the increasingly diverse world around us and strive to create an empowering and welcoming workplace culture. We are a $4.0 billion publicly traded global manufacturer of materials processing and aerial work platform products and services. We are passionate about producing equipment that helps improve the lives of people around the world and providing our team members with a rewarding career and the opportunity to make an impact.
-While our operations are global, each office or factory is a close-knit community. We value diversity, equity and inclusion, safety, integrity, respect, servant leadership, courage, citizenship, and continuous improvement. It's an exciting time to be part of the expanding manufacturing sector - come join us!
-We see inclusion as a key to our success and are committed to actively foster a culture where every team member feels valued, listened to, and appreciated. We are committed to being fair and impartial in our decisions, ensuring equity within our workplace. As an Equal Opportunity Employer, employment decisions are made without regard to race, color, religion, national or ethnic origin, sex, sexual orientation, gender identity or expression, age, disability, protected veteran status or other characteristics protected by law.
-Globaltalentacquisitions@terex.com
-The Company offers competitive salaries, advancement opportunities, and a full range of benefits, including paid vacation, 401(k), medical, dental, and vision.
-Terex Corporation is an Equal Opportunity Employer and Affirmative Action Employer M/F/D/V.</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Machinery Manufacturing</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
- Tratamento pra caso algum campo não exista, não travar execução.
</commit_message>
<xml_diff>
--- a/data/jobs_information.xlsx
+++ b/data/jobs_information.xlsx
@@ -514,34 +514,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RPA Engineer - Remote Work</t>
+          <t>Product Owner with RPA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Who We are
-BairesDev is proud to be the fastest-growing company in America. With people in five continents and world-class clients, we are only as strong as the multicultural teams at the heart of our business. To consistently deliver the highest quality solutions to our clients, we only hire the Top 1% of the best talents and nurture their professional growth on exciting projects.
-RPA Engineer at BairesDev
-We are looking for an RPA Engineer to join our Development Team. In this position, you will work with cross-functional teams and business analysts to optimize and automate business processes with RPA technologies, ensuring the automation follows best practices, scalability, and easy maintenance.
-How we do make your work (and your life) easier:
-Our people work remotely but with a consistent and robust culture that promotes diversity and teamwork. To continue being the leading software development company in Latin America, we want to ensure that every BairesDev member gets the best growth and professional development opportunities in a diverse, welcoming, and innovative environment.
-Every BairesDev team member brings something unique to our company.
-We want to hear your story. Apply now!</t>
+          <t>Company Overview
+Cloud BC Labs Inc is a digital transformation organization aimed at creating seamless solutions for clients to effectively manage their business operations. The company specializes in Business and Management Consulting, AI/ML, Data Analytics &amp; Visualization, Cloud Data Warehouse Migration, Snowflake Implementation, Informatica Implementation &amp; Upgrade, Staffing Services and Data Management Solutions.
+RPA Product Manager will be responsible for delivering high-quality RPA solutions understanding the different requirements from internal teams and driving service adoption. Standard work includes: Lead the UiPath product lifecycle management including release planning, knowledge creation, used case documentation, product launch and post go-live support. Accountable for Infosec and service transition activities of new RPA products. Drive product marketing to improve the service adoption of new UiPath Products. Determine RPA best practices and drive improvements on current processes, standards and practices within the organization. Proactively identify and escalate security and privacy risks/issues as a Product Manager. Design and build RPA training workshops and deliver this at enterprise level. Contribute and maintain our RPA CoE (Center of Excellence) site. Represent Global Services RPA CoE internal discussion boards and providing guidance to internal EY RPA users. Maintain documentation according to firm standards, best practices, and standard operating procedures.
+Cloud BC Labs Inc is a digital transformation organization aimed at creating seamless solutions for clients to effectively manage their business operations. The company specializes in Business and Management Consulting, AI/ML, Data Analytics &amp; Visualization, Cloud Data Warehouse Migration, Snowflake Implementation, Informatica Implementation &amp; Upgrade, Staffing Services and Data Management Solutions</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Entry level</t>
+          <t>Mid-Senior level</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Engineering and Information Technology</t>
+          <t>Product Management and Marketing</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -556,19 +552,38 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>UI Path - RPA Developer</t>
+          <t>RPA Developer</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Role : UI Path_RPA Developer
-Location : 100% remote
-Job Description</t>
+          <t>Company Overview
+Spry brings a unique blend of proven service delivery, scalable and agile corporate infrastructure, and the ability to recruit and retain the best and brightest in the industry to support our customers. The Spry team engages in exciting and rewarding opportunities that challenge their abilities, in an atmosphere that encourages both personal and professional growth, fostering a positive and energetic work environment.
+Who We're Looking For (Position Overview):
+Spry Methods is on the search for a Senior Level UI Path RPA developer. This position will support Enterprise Resource Planning Office within the Naval Research Laboratory. Candidates’ main responsibility will be serving as a Robotic Process Automation (RPA) Developer responsible for creating automations across the Comptroller and Business community.
+What Your Day-To-Day Looks Like (Position Responsibilities):
+Candidate will be expected to interact with customers/peers from across the organization and must be comfortable interacting with peers in different departments. This is a challenging position, and the ideal candidate is a quick learner with an excellent work ethic and strong technical aptitude. The candidate must be able provide timely and accurate work products to support team and customer deadlines. An ability to work effectively both independently and in a supportive, diverse team environment is expected.
+What You Need to Succeed (Minimum Requirements):
+Ideally, You Also Have (Preferred Qualifications):
+Perks of Working for Us (Benefits):
+Medical Coverage – United Healthcare - 3 Options
+Vision Coverage – VSP - Vision Service Plan
+Dental Coverage – Guardian Dental - PPO Premier Plan or Value Plan
+Paid Holidays: Full-time employees receive 11 paid federal holidays
+Paid Time Off (PTO) – PTO accrural starts at 15 days per year
+Training Benefit – Annual training allowance available toward any job-related training or education
+401 (k) – Multiple Fund Choices through Professional Capital Service (PCS) with a company match
+For our full list of benefits, please visit http://www.sprymethods.com/careers/benefits/
+COVID-19 Vaccination Requirement
+The COVID-19 vaccination requirement stated in Executive Order 14042 and FAR 52.223-99 is currently not implemented, however, please note that if E.O. 14042 or other related requirements become effective, positions will require successful candidates/employees to obtain and show proof of COVID-19 vaccination(s). Spry is an equal opportunity employer and will provide reasonable accommodation to those individuals who are unable to be vaccinated consistent with federal, state, and local law.
+EEO Statement
+At Spry, we believe talented and dedicated employees are our most valued assets and the foundation of our success. We are committed to crafting a diverse and inclusive workplace that endorses engagement, creativity, quality and innovation.
+We are proud to be an Affirmative Action and Equal Opportunity Employer and as such, we evaluate qualified candidates in full consideration without regard to race, color, religion, sex, sexual orientation, gender identity, marital status, national origin, age, disability status, protected veteran status, and any other protected status.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Entry level</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -583,7 +598,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Human Resources</t>
+          <t>Information Technology &amp; Services</t>
         </is>
       </c>
     </row>
@@ -598,15 +613,21 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Description
-"You've worked for the rest...now work for the best!"
-Trinity Solar...recognized by NJ Biz as one of the top 250 private companies in 2022.
-Trinity Solar...recognized as a top 2022 Solar Contractor by Solar world.
-The RPA Developer is responsible for developing, integrating, testing, and maintaining existing and new RPA-based solutions. They will work closely with the RPA team and Business Technology department by writing code using RPA software as well as Python language to develop these solutions.
-Not just a career... but a career path to success! Trinity Solar offers you a career in one of the fastest growing fields in the country. A career with Trinity Solar is a path to personal and professional growth with a company who truly values its employees. Our employees enjoy...
-Since 1994, Trinity Solar has proudly provided energy with integrity to families in our area. Trinity started in the solar industry with two core fundamental principles, to make renewable energy accessible and to make the solar journey seamless. These guiding beliefs have led Trinity Solar to become the United States largest privately-held residential solar installer, composed of more than 1,700 team members and boasting over 70,000 installations. Currently, Trinity offers solar installation in Connecticut, Delaware, Florida, New Jersey, New York, Massachusetts, Maryland, Pennsylvania, and Rhode Island.
-Trinity Solar is an Equal Opportunity Employer committed to diversity in the workplace. Consistent with that goal, all qualified applicants will receive consideration for employment without regard to race, color, religion, sex, sexual orientation, national origin, age, disability, protected veteran status, gender identity, or any other category protected by applicable federal, state, or local laws.
-"Veteran Friendly"</t>
+          <t>TECHNOGEN, Inc. is a Proven Leader in providing full IT Services, Software Development and Solutions for 15 years.
+TECHNOGEN is a Small &amp; Woman Owned Minority Business with GSA Advantage Certification. We have offices in VA; MD &amp; Offshore development centers in India. We have successfully executed 100+ projects for clients ranging from small business and non-profits to Fortune 50 companies and federal, state and local agencies.
+Position: Sr. RPA Developer (UiPath)
+Location: Trenton, NJ(Hybrid)
+Duration: Long Term
+UIPath Certification Required
+We are seeking Senior RPA developer / designer for leading, designing and delivering RPA solutions in accordance with industry standards and best practices. Experience in COMPLEX (not basic) Automation experience is required.
+A Senior RPA developer / designer for leading, designing and delivering RPA solutions in accordance with industry standards and best practices. Candidate will work closely together with our enthusiastic team of both business and technical specialists. Judiciary RPA environment includes UIPath and PEGA Robotics. As part of a fast-growing and successful team that helps our business get the maximum benefit, candidates will lead workshops and interviews with business process SMEs to gather and optimize business process details, create PDDs, develop POCs, pilots and production automation.
+,
+Ashok Kumar
+Sr. Talent Acquisition Specialist
+Phone: 443-832-6103
+Email: ashok.c@technogeninc.com
+Web: www.technogeninc.com
+4229 Lafayette Center Dr, Suite 1880, Chantilly, VA 20151</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -616,7 +637,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -626,7 +647,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Renewable Energy Semiconductor Manufacturing</t>
+          <t>IT Services and IT Consulting</t>
         </is>
       </c>
     </row>
@@ -636,37 +657,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RPA Analyst</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Company Description
-ClientSolv Technologies is an IT solution firm with over a decade of experience serving Fortune 1000 companies, public sector and small to medium sized companies. ClientSolv Technologies is a woman-owned and operated company that is certified as a WMBE, 8a firm by the Federal government's Small Business Administration.
-We are seeking an RPA Analyst for a direct hire/permanent role. This role can work remotely within the following states: Arkansas, Colorado, Illinois, Indiana, Iowa, Kansas, Kentucky, Minnesota, Missouri, Montana, Nebraska, New Mexico, North Dakota, Oklahoma, South Dakota, Tennessee, Texas, and Virginia.
-Day to day this person will be
-Bachelor's Degree in accounting, finance, management information systems, computer and information science. Technical business master’s degree such as M.S. of Finance preferred.
-Additional Information</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mid-Senior level</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Engineering and Information Technology</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>IT Services and IT Consulting</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -676,22 +692,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RPA Analyst</t>
+          <t>E- Retail Manager</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>Company Description
-ClientSolv Technologies is an IT solution firm with over a decade of experience serving Fortune 1000 companies, public sector and small to medium sized companies. ClientSolv Technologies is a woman-owned and operated company that is certified as a WMBE, 8a firm by the Federal government's Small Business Administration.
-We are seeking an RPA Analyst for a direct hire/permanent role. This role can work remotely within the following states: Arkansas, Colorado, Illinois, Indiana, Iowa, Kansas, Kentucky, Minnesota, Missouri, Montana, Nebraska, New Mexico, North Dakota, Oklahoma, South Dakota, Tennessee, Texas, and Virginia.
-Day to day this person will be
-Bachelor's Degree in accounting, finance, management information systems, computer and information science. Technical business master’s degree such as M.S. of Finance preferred.
-Additional Information</t>
+LVMH Fragrance Brands is a house of the Perfumes and Cosmetics division of LVMH Group. It was created in 2011 and brings together the savoir-faire and the passion of two iconic brands: Parfums Givenchy and Kenzo Parfums.
+For more than 60 years has perpetuated the values of its founder, Hubert de Givenchy, releasing fragrances, makeup and skincare products that define free, assertive, and bold women.
+Parfums Givenchy fragrances embody the brand’s Fearless Classic vision, fusing genres and revealing unexpected twists. Inspired by the avant-garde spirit and sensuality of Givenchy Couture creations, Nicolas Degennes, Makeup and Color Artistic Director since 1999, continues to reveal the inventiveness synonymous with Givenchy.
+In 1970, Takada instilled a touch of jungle exoticism at the heart of Paris, in Galerie Vivienne. With his colorful prints and his self-professed creative freedom, Kenzo upturned the couture diktats of the time by merrily breaking the rules.
+The brand’s first feminine fragrance, called Kenzo, was born in 1988. Then followed a series of creations with a unique and original identity that made a strong impression on the world of perfumery. They all tell an optimistic story and play with a mix of multicultural codes to savor again and again. The bottles themselves are symbols of pure refinement and emblems of the brand’s values.
+LVMH Fragrance Brands invites you today to join its North America teams.
+LVMH Fragrance Brands is part of the LVMH Group.
+Responsible for sales, marketing activation, business planning and execution for E-retail channel (select accounts).
+Develop &amp; implement sound strategies for online promotional &amp; marketing activities, product assortment &amp; information, Retailer CRM, &amp; digital programs to increase revenue &amp; profit while maintain a cohesive dotcom presence.
+:
+Develop the strategy and conduct planning and execution of product information, online advertising, and promotions for continued growth of LVMH Fragrance Brands products on partner E-Retailer sites.
+This role includes the planning of all e-retail business (sales plan, marketing activities, content calendars, coop) for each retailer.
+Ensure that the image of the brand is consistent across all retailer execution.
+:
+Senior Manager E-Business
+Manage E-Retail Coordinator and intern to help achieve E-Retail and Business Goals
+Thought-leader on indirect e-business for broader team
+Additional Information
+All your information will be kept confidential according to EEO guidelines.
+Salary range $90-100k</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Mid-Senior level</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -701,12 +732,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Engineering and Information Technology</t>
+          <t>Sales and Business Development</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>IT Services and IT Consulting</t>
+          <t>Personal Care Product Manufacturing</t>
         </is>
       </c>
     </row>
@@ -716,377 +747,10 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RPA Product &amp; Engineering Lead</t>
+          <t>Remote UiPath Robotics Process Automation Engineer (RPA) - Remote | WFH</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
-        <is>
-          <t>At Disney, we’re storytellers. We make the impossible, possible. The Walt Disney Company is a world-class entertainment and technological leader. Walt’s passion was to continuously envision new ways to move audiences around the world—a passion that remains our touchstone in an enterprise that stretches from theme parks, resorts and a cruise line to sports, news, movies and a variety of other businesses. Uniting each endeavor is a commitment to creating and delivering unforgettable experiences — and we’re constantly looking for new ways to enhance these exciting experiences.
-The Enterprise Technology mission is to deliver technology solutions that align to business strategies while enabling enterprise efficiency and promoting cross-company collaborative innovation. The Enterprise Technology organization drives competitive advantage by enhancing our consumer experiences, enabling business growth, and advancing operational excellence.
-The Data Solutions &amp; Platforms team is responsible for developing data &amp; analytics solutions for business groups across the enterprise. We are a collaborative engineering team who enjoy delivering innovative solutions to complex business challenges. Examples of platforms and services we are responsible for include: data integration hub, data warehouses, BI tools, data science tools, Robotic Process Automation (RPA) and other automation tools.
-The RPA Product &amp; Engineering Lead role will have the following responsibilities:
-The hiring range for this position in California is $149,240 to $200,200 per year and in Washington State is $156,292 to $209,660 per year. The base pay actually offered will take into account internal equity and also may vary depending on the candidate’s geographic region, job-related knowledge, skills, and experience among other factors. A bonus and/or long-term incentive units may be provided as part of the compensation package, in addition to the full range of medical, financial, and/or other benefits, dependent on the level and position offered.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Information Technology</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Entertainment Providers</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>RPA Consultant</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Job Description
-Role RPA Consultant
-Locations Plano, TX
-Bachelors degree in Computer Science, Engineering, Information Technology or related area
-8&amp;plus; years experience in Distributed Multi-tier Application Development and Robotics Process Automation
-Advanced experience working with Automation tools-Winautomation (Primary) or (secondary) Automation Anywhere
-Strong ASP.NET MVC, .NET Core and/or Java Object Oriented programming experience including significant understanding of HTML, CSS, AJAX, JavaScript, VBA, Xpath, XML, JSON, React, Bootstrap, JSF, Spring MV, and Angular frameworks.
-Strong foundation of database development with Oracle
-Experience working on Test driven development environment and Java testing frameworks such as Build test cases using automated testing .NET and/or Java frameworks (MSTest, NUnit, XUnit, Unit Test, Junit,Mocks etc.)
-Knowledge on various DevOps key concepts and CI/CD tools such as JIRA, Bitbucket, Jenkins etc.
-Experience at service oriented application development and integration within cloud platform such as AWS or similar.
-Strong experience on best architecture practices for Microservices and data modeling.
-Working experience as Agile developer and good understanding of SDLC methodologies/guidelines
-2-3 years of Mortgage/Banking/finance analytical support experience preferred, but not mandatory.
-Optional experience with Tableau BI tool
-Added experience of using Python for Web development frameworks is a plus.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>RPA Consultant</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Job Description
-Role RPA Consultant
-Locations Plano, TX
-Bachelors degree in Computer Science, Engineering, Information Technology or related area
-8&amp;plus; years experience in Distributed Multi-tier Application Development and Robotics Process Automation
-Advanced experience working with Automation tools-Winautomation (Primary) or (secondary) Automation Anywhere
-Strong ASP.NET MVC, .NET Core and/or Java Object Oriented programming experience including significant understanding of HTML, CSS, AJAX, JavaScript, VBA, Xpath, XML, JSON, React, Bootstrap, JSF, Spring MV, and Angular frameworks.
-Strong foundation of database development with Oracle
-Experience working on Test driven development environment and Java testing frameworks such as Build test cases using automated testing .NET and/or Java frameworks (MSTest, NUnit, XUnit, Unit Test, Junit,Mocks etc.)
-Knowledge on various DevOps key concepts and CI/CD tools such as JIRA, Bitbucket, Jenkins etc.
-Experience at service oriented application development and integration within cloud platform such as AWS or similar.
-Strong experience on best architecture practices for Microservices and data modeling.
-Working experience as Agile developer and good understanding of SDLC methodologies/guidelines
-2-3 years of Mortgage/Banking/finance analytical support experience preferred, but not mandatory.
-Optional experience with Tableau BI tool
-Added experience of using Python for Web development frameworks is a plus.</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RPA Consultant</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Job Description
-RPA Consultant
-Hockessin, DE</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>RPA Consultant</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Job Description
-Role: RPA Consultant
-Location: Austin, TX
-Experience: 4-6 Year
-Duration: 6-12 Months</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>RPA CONSULTANT</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Job Description
-RPA Consultant
-Syracuse, NY</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>RPA Technical Analyst</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>We are seeking a Robotic Process Automation (RPA) Technical Analyst to join a larger team that supports our Federal customer in the identification and automation of Momentum processes. The RPA Technical Analyst will follow the full lifecycle of development and deployment of processes to be automated. Candidates should have familiarity with Federal financials, experience with Momentum is preferred. This is a full-time position on a multi-year contract that will allow for remote work with occasional on-site client meetings in Washington, DC.
-All employment decisions shall be made without regard to age, race, creed, color, religion, sex, national origin, ancestry, disability status, veteran status, sexual orientation, gender identity or expression, genetic information, marital status, citizenship status or any other basis as protected by federal, state, or local law.</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Entry level</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Information Technology</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Technology, Information and Internet</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>RPA Engineer</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Job Description
-Title: RPA Engineer
-Location: New York, NY</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Entry level</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>RPA (Robotic Process Automation)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Job Description
-!! Greetings !!
-My name is Abdul and I'm a Team Lead at Diverse Lynx. We provide IT Consulting Services to our customers' immediate and long-term resource needs. I am contacting you either because your resume has been posted to one of the internet job sites to which we subscribe or you had previously submitted your resume to . We now find your resume matching for a opportunity with our client at
-Automation Anywhere Certified Advanced RPA professional(V10&amp; V11)
-Prior RPA experience is strongly preferred. Experience setting up RPA COEs a plus
-5&amp;plus; years of professional services experience working directly with clients, on automation and/or integration projects
-Strong working knowledge of infrastructure and datacenter concepts such as HA, DR, virtualization, networking, load balancing, etc.
-Excellent communication skills both verbal and written, and comfortable presenting materials across multiple levels of the organization. Must have strong technical knowledge and analytical skills.</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Entry level</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Remote UiPath Robotics Process Automation Engineer (RPA) - Remote | WFH</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
         <is>
           <t>Are you ready to join a dynamic team and revolutionize the way our government customer/MBS provider agency operates? We're looking for a talented RPA Engineer to develop cutting-edge Robotic Process Automation (RPA) solutions, including Artificial Intelligence (AI), Cognitive Computing/Machine Learning (ML), and Chatbots. In this role, you'll have the opportunity to work in an agile software development environment and make a real impact.
 As an RPA Engineer, you will be responsible for supporting the development and management of all operational bots. You'll assess the suitability of use cases and optimize processes, develop and test bots, provide chatbot proof-of-concepts, and monitor the performance and security of the digital workforce.
@@ -1099,24 +763,382 @@
 So, are you ready to take on this exciting challenge and make a difference? Apply now!</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Human Resources Services</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>RPA Scrum Master</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Job Description
+Title: RPA Developer
+Locations Remote
+Experienced, highly collaborative Business Systems Analyst with knowledge and experience in Robotic Process Automation using UiPath
+Experience with Robotics Process Automation tools [e. g., Automation Anywhere, UI Path, Open Span, Block Chain, and Natural Language Processing (NLP)].
+Experience with applications such as LucidChart, Confluence, JIRA, and/or Smartsheet.
+Domain knowledge and or experience with Financial and Legal enterprise applications and processes is preferred
+Experience with Agile methodologies
+Should be flexible, self-driven, detail oriented and analytical
+Drive cross functional E2E projects all the way from defining scope, eliciting requirements, development, testing and launch
+Translate business objectives and customer needs into clearly written business requirements
+Determine the right technology to fit the business requirements. Partner with various business and technical teams to drive the implementation of strategic initiatives
+Regularly communicate relevant changes/updates to the internal stakeholders
+Create and maintain pertinent documentation
+Apply excellent interpersonal skills across multiple organizations; communicate effectively to technical and non-technical stakeholders
+Configuration setup, end-to-end testing, and maintenance of RPA, Finance and Legal systems /applications</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Mid-Senior level</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Contract</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Business Intelligence Analyst</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Overview
+Exaktera is a leading industrial technology manufacturing company focused on delivering innovative, market driven, light-based OEM components and sub-systems to meet the illumination, sensing, detection and imaging needs of our customers. We are uniting widely recognized and respected brands in critical light-based technology solutions for leading OEM customers in both industrial and medical end markets. Our global customers rely on the highest performing laser and LED technologies in combination with our deep applications expertise to improve the quality, safety and production efficiency of their manufacturing operations. Exaktera is a global entity with multiple offices in the United States and Europe.
+As a Business Intelligence Analyst (“BIA”), your insights will play a central role in developing the end-to-end strategy of Exaktera and supporting the executive and business teams as we create and grow Exaktera. You will work closely with the C-Suite, Board of Directors and key leaders throughout the business to create real time insights into the performance of the business while providing trend analysis to unlock further growth via the combined views of each of our acquired brands. This newly created role would ideally be based out of one of our U.S. operating sites in , or based at one of our manufacturing sites in . Discretionary consideration may be given for remote work elsewhere for the right candidate. The position will report to the CFO of Exaktera.
+A successful data migration initiative is at the center of this role. The ideal candidate for this position will be a self-starter, self-managed, problem-solver and capable of handling multiple tasks and projects in a fast-paced environment. The BIA will be the bridge, working with all stakeholders and global operating sites to implement, consolidate and prioritize key metrics, then help guide business decisions for improving processes, products, and solutions as we continue to grow organically and through acquisitions.
+Powered by JazzHR
+pjSDjNveRT</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Mid-Senior level</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Research, Analyst, and Information Technology</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Internet Publishing</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RPA Developer- Hybrid- Houston, TX</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Interested in working for a company that brings the power of energy to people and organisations by putting customers at the center of everything they do? If so, this company might be for you!
+Responsibilities</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Staffing and Recruiting</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>RPA Engineer - Remote Work</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Who We are
+BairesDev is proud to be the fastest-growing company in America. With people in five continents and world-class clients, we are only as strong as the multicultural teams at the heart of our business. To consistently deliver the highest quality solutions to our clients, we only hire the Top 1% of the best talents and nurture their professional growth on exciting projects.
+RPA Engineer at BairesDev
+We are looking for an RPA Engineer to join our Development Team. In this position, you will work with cross-functional teams and business analysts to optimize and automate business processes with RPA technologies, ensuring the automation follows best practices, scalability, and easy maintenance.
+How we do make your work (and your life) easier:
+Our people work remotely but with a consistent and robust culture that promotes diversity and teamwork. To continue being the leading software development company in Latin America, we want to ensure that every BairesDev member gets the best growth and professional development opportunities in a diverse, welcoming, and innovative environment.
+Every BairesDev team member brings something unique to our company.
+We want to hear your story. Apply now!</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>IT Services and IT Consulting</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RPA Technical Lead</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Concentrix Catalyst is the experience design and engineering team of Concentrix, a leading global solutions company that reimagines everything CX through strategy, talent and technology. We combine human-centered design, powerful data and strong tech to accelerate CX transformation at scale.
+The Catalyst Team is seeking an RPA Technical Lead to join our full-time team as full-time employee.
+In order to provide equal employment and advancement opportunities to all individuals, employment decisions at Concentrix Catalyst are based exclusively on merit. Concentrix Catalyst does not discriminate in employment opportunities or practices on the basis of race, color, religion, sex, including gender identity and identity expression, national origin, age, or any other characteristic protected by law.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Mid-Senior level</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>IT Services and IT Consulting</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Automation Support Lead</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Accelirate Automation Support Leads are trained in Robotic Process Automation tools and methodologies.
+Incoming members go through a structured training program which will teach them the fundamentals of process automation, introduce them to specialized RPA topics, and prepare them for end-to-end client automation.
+This is a team of motivated, and energetic individuals that participate in the process of design, coding, unit testing, and debugging of new robots based on Accelirate’s proprietary methodology.
+Essential Duties Include:
+Minimum Degree Requirement:
+Bachelor’s Degree in a Computer Science, Software Engineering, or Related Disciplines.
+Powered by JazzHR
+eXMiYFZroI</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Internship</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Internet Publishing</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Robotic Process Automation (RPA) developer</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>AVER is seeking a motivated Robotic Process Automation (RPA) developer with strong technical knowledge and great communication and problem-solving skills to support a long-term program in the OCFO for our Homeland Security client. The project mission is to increase data-driven decisions by developing and integrating analytical tools and automating related processes across multiple tasks and financial models.
+AVER, LLC is a Data &amp; Digital Transformation company that delivers exceptional client service with great people and transformative technology solutions to enable Government mission success. We provide customers with specialized technical skills and deep subject matter expertise focused on Homeland Security, Biometrics, Law Enforcement and Healthcare domains to meet the complex mission challenges today and tomorrow. We are a verified Service-Disabled Veteran-Owned Small Business (SDVOSB) that strives to provide a customer-centric experience building trusted partnerships with our clients and people.
+Powered by JazzHR
+K4XRmdH5RK</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Mid-Senior level</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Engineering and Information Technology</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Internet Publishing</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>RPA Analyst</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Excellent opportunity to join NRG, an industry-leading Fortune 200 company with more than 6,500 employees providing energy solutions and natural gas to more than six million customers across the United States and Canada! With robust training programs and skill development, NRG offers opportunities for career advancement while working toward a sustainable energy future.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Associate</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Engineering, Information Technology, and Analyst</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Renewable Energy Semiconductor Manufacturing, Oil and Gas, and Utilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>RPA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Job Description
+TITLE:. RPA consultant
+LOCATION :: Chicago, IL (Remote Until Covid)
+: 6 &amp;plus; Years</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Entry level</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Engineering and Information Technology</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Human Resources Services</t>
+          <t>Software Development</t>
         </is>
       </c>
     </row>
@@ -1126,30 +1148,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RPA PM</t>
+          <t>RPA Consultant</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>Job Description
-Job Title: RPO PM
-Location: Atlanta, GA(Remote until covid-19 restriction left)
-Duration: Contract-to-Hire</t>
+RPA Consultant
+Hockessin, DE</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Entry level</t>
+          <t>Mid-Senior level</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Project Management and Information Technology</t>
+          <t>Engineering and Information Technology</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1164,15 +1185,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RPA PM</t>
+          <t>RPA QA role</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>Job Description
-RPA PM
-Location is Boston, MA
-The PM position requires and MAPD knowledge is nice to have.</t>
+Role : Quality Analyst
+Location : Remote for 2022 , Client preferred locations – Charlotte, NC / St.Louis,MO
+Relevant Experience (Years): 4&amp;plus; Years</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1182,12 +1203,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Contract</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Project Management and Information Technology</t>
+          <t>Quality Assurance</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1202,20 +1223,18 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Automation Engineer</t>
+          <t>RPA Developer</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Job Details
-Description
-About Canal Insurance
-Canal Insurance Company was founded in 1939 and is located in Greenville, South Carolina. Canal specializes in insurance for commercial trucking and specialty transportation operations. While Canal does not write insurance in all states, the claims department handles claims in all 48 contiguous states and Canada. Canal’s customers are mainly federally regulated Motor Carriers and as such the core group of customers carry $1,000,000 in liability limits.
-At Canal, we recognize that our success would not be possible without the hard work and dedication of our employees. We know that happiness and productivity go hand in hand, and to that end, we consciously cultivate a culture that enables us to recruit and retain the very best talent in the business.
-The Automation Engineer will be responsible for designing, developing, and implementing automation solutions to improve efficiency and productivity in the development, testing, and deployment of software applications. You will also work with IT and Business cross-functional teams to identify opportunities for automation and implement solutions to meet those needs.
-Bachelor’s degree in business, computer science, engineering or related field, or related years of experience
-Constant use of vision, hearing, and communication (oral and written in person and via telephone). Frequent concentration, standing, walking, handling, reaching, and grasping. Occasional bending, kneeling and lifting (up to 25 lbs.) Heavy use of computer and office equipment.
-Occasional travel may be required. Periodic work outside of standard business hours or on weekends may be required.</t>
+          <t>Description
+Background:
+IT Concepts (ITC) is an 8(a) SDVOSB founded on the concepts of customer-centric, driven to deliver, teamwork, integrity, and innovation. Founded in 2003, ITC was established with a simple yet important promise to “deliver solutions that work”. As we continue to grow in the support of our government customers, we are looking for driven and innovative individuals to join our team.
+IT Concepts is seeking a RPA Developer who will support several projects at a federal agency. The position is located in Woodlawn, MD. The qualified candidate should have strong analytical, problem-solving, and communication skills with sharp attention to detail.
+At least 5 to 7 years of experience is required with a Technical Bachelor’s Degree or 3 to 5 years of experience is required with a Master’s Degree.
+UIPath certifications desired but not required.
+Ability to be able to pass a Federal government Public Trust Clearance</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1235,7 +1254,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Insurance</t>
+          <t>IT Services and IT Consulting</t>
         </is>
       </c>
     </row>
@@ -1245,36 +1264,33 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UIPath Developer - RPA Developer</t>
+          <t>Data Scientist</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Position: UIPath Developer - RPA Developer
-Location: Alameda, CA ( onsite only)
-Position Type: Full-time Employee or contract
-Be a part of the Operations team focusing on Robotics process automation maintenance Monitoring RPA tool (UiPath)
-We offer a competitive salary, benefits, and a dynamic work environment. If you have a passion for technology and are looking for an exciting opportunity to work with a talented team, please apply today</t>
+          <t>SOCOM CDO – Tampa, FL – Top Secret Clearance Required
+STEMBoard is seeking a data scientist with knowledge in programming for integrating complex models and using advanced software library frameworks to distribute large, clustered data sets. The data scientist work with a team of data scientists and engineers that collect and arrange data in a form that is useful for analytics. A knowledge of machine learning is also desired to build efficient and accurate data pipelines to meet the needs for downstream users such as data scientists to create the models and analytics that produce insight.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Entry level</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Contract</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Engineering and Information Technology</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Information Technology &amp; Services</t>
+          <t>Technology, Information and Internet</t>
         </is>
       </c>
     </row>
@@ -1284,10 +1300,118 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Business Intelligence Analyst</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Overview
+Exaktera is a leading industrial technology manufacturing company focused on delivering innovative, market driven, light-based OEM components and sub-systems to meet the illumination, sensing, detection and imaging needs of our customers. We are uniting widely recognized and respected brands in critical light-based technology solutions for leading OEM customers in both industrial and medical end markets. Our global customers rely on the highest performing laser and LED technologies in combination with our deep applications expertise to improve the quality, safety and production efficiency of their manufacturing operations. Exaktera is a global entity with multiple offices in the United States and Europe.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Mid-Senior level</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Research, Analyst, and Information Technology</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Venture Capital and Private Equity Principals</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>RPA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Title……. RPA
+Location……… Mclean, VA
+Job Type Contract/Fulltime….. Contract or Full Time</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Entry level</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Contract</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>IT Services and IT Consulting</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Continuous Improvement Analyst</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Excellent opportunity to join NRG, an industry-leading Fortune 200 company with more than 6,500 employees providing energy solutions and natural gas to more than six million customers across the United States and Canada! With robust training programs and skill development, NRG offers opportunities for career advancement while working toward a sustainable energy future.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Associate</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Engineering, Information Technology, and Analyst</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Renewable Energy Semiconductor Manufacturing, Oil and Gas, and Utilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>RPA BA</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Job Description
 Role: RPA BA
@@ -1308,147 +1432,19 @@
 Configuration setup, end-to-end testing, and maintenance of RPA, Finance and Legal systems /applications</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Mid-Senior level</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>Full-time</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Research, Analyst, and Information Technology</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>RPA BA</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Job Description
-Role: RPA BA
-Location : Mountain View, CA ( relocation post covid)
-Pay Rate : $42/hr on w2 (Slightly Negotiable)
-JD
-Experienced, highly collaborative Business Systems Analyst with knowledge and experience in Robotic Process Automation using UiPath
-Experience with Robotics Process Automation tools [e. g., Automation Anywhere, UI Path, Open Span, Block Chain, and Natural Language Processing (NLP)].
-Experience with applications such as LucidChart, Confluence, JIRA, and/or Smartsheet.
-Domain knowledge and or experience with Financial and Legal enterprise applications and processes is preferred
-Experience with Agile methodologies
-Should be flexible, self-driven, detail oriented and analytical
-Drive cross functional E2E projects all the way from defining scope, eliciting requirements, development, testing and launch
-Translate business objectives and customer needs into clearly written business requirements
-Determine the right technology to fit the business requirements. Partner with various business and technical teams to drive the implementation of strategic initiatives
-Regularly communicate relevant changes/updates to the internal stakeholders
-Create and maintain pertinent documentation
-Apply excellent interpersonal skills across multiple organizations; communicate effectively to technical and non-technical stakeholders
-Configuration setup, end-to-end testing, and maintenance of RPA, Finance and Legal systems /applications</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Research, Analyst, and Information Technology</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>RPA BA</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Job Description
-RPA BA
-Remote
-Contract</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Mid-Senior level</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Research, Analyst, and Information Technology</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Robotic Process Automation (RPA) BA</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Job Description
-Role Robotic Process Automation (RPA) BA
-Location Bentonville, AR (Remote until COVID-19 restrictions lift)
-Duration 6 months (Contract to hire after 6 months)</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Entry level</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Engineering and Information Technology</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1463,23 +1459,52 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Data Scientist</t>
+          <t>Applications Programmer RPA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>SOCOM CDO – Tampa, FL – Top Secret Clearance Required
-STEMBoard is seeking a data scientist with knowledge in programming for integrating complex models and using advanced software library frameworks to distribute large, clustered data sets. The data scientist work with a team of data scientists and engineers that collect and arrange data in a form that is useful for analytics. A knowledge of machine learning is also desired to build efficient and accurate data pipelines to meet the needs for downstream users such as data scientists to create the models and analytics that produce insight.</t>
+          <t>Duties / Responsibilities:-
+Demonstrate strong knowledge of Robotic Process Automation (RPA) development methodologies, prototyping, business process analysis for automation, automating user flows, innovative solutions, and performing associated coding.
+Translate business process workflows into automated solutions requirements.
+Understand, define, and analyze business processes for automation.
+Design and code Bots using various automation tools in UiPath and other equivalent technologies.
+Evaluate and test workflows, perform human-in-the-loop functions, and debug, deploy, maintain, document, and implement complex business workflow automation.
+Deploy RPA components, including bots, development tools, code repositories, and logging tools.
+Support the launch and implementation of RPA solutions.
+Create process and end-user documentation.
+Work with business, technical, non-technical, and cross-functional resources to define and deliver business-impacting automation solutions.
+Work directly with stakeholders to capture business requirements and translate them into technical approaches and designs that can be implemented.
+Maintain current knowledge of relevant technologies and business processes.
+Develop and execute automated test scenarios and integration plans/scripts to validate the workflow automation changes meeting technical specifications and business requirements.
+Work with business teams to complete acceptance testing and participate in integration testing.
+Adhere to all security, change control, and MHBE Project Management Office (PMO) policies, processes, and methodologies.
+A minimum of four (4) years of experience in any programming languages such as C/C++, Python, VB Script, Ruby, Java, JS, .Net developing enterprise applications.
+A minimum of two (2) years of hands-on experience with Robotic Process Automation (RPA) tools and cognitive platforms such as UiPath, Blue Prism, Automation Anywhere, etc.
+A minimum of two (2) years of experience utilizing HTML, JavaScript, or any scripting language.
+Proven ability to design technical specification documents for RPA Projects.
+Experience developing and consuming APIs for large systems.
+Experience with Agile development methodology.
+Knowledge of artificial intelligence and machine learning applied in an enterprise setting automating business or technical workflows.
+Strong attention to detail and analytical skills.
+Knowledge of Agile software development practices
+A minimum of four (4) years of hands-on experience with UiPath or equivalent, automating complex workflows for an enterprise application or business process.
+Experience with SQL or NoSQL databases, performing data analysis related to workflow automation.
+Proven experience in understanding business process workflows and identifying opportunities for automation.
+Experience utilizing RPA in a Cloud environment.
+Experience working in an Agile software development environment.
+UiPath RPA Developer or RPA Associate certification.
+Experience working with the Project Management Office (PMO) processes, policies, and procedures.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1489,7 +1514,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Technology, Information and Internet</t>
+          <t>Public Relations and Communications Services and Government Relations Services</t>
         </is>
       </c>
     </row>

</xml_diff>